<commit_message>
Update data file and read multiple sheets
</commit_message>
<xml_diff>
--- a/data/market_data.xlsx
+++ b/data/market_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="mexico_market_size" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
     <sheet name="usa_market_share" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="usa_channel_breakdown" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="category_definitions" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="channel definitions" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="channel_definitions" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -322,6 +322,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -344,6 +345,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Aril"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -351,6 +353,7 @@
       <color rgb="FF595959"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -359,12 +362,14 @@
       <color rgb="FF595959"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF595959"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -372,6 +377,7 @@
       <color rgb="FF595959"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -514,7 +520,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -759,6 +765,10 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -839,11 +849,11 @@
   </sheetPr>
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2324,7 +2334,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2636,7 +2646,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3364,7 +3374,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4845,7 +4855,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5317,7 +5327,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6045,192 +6055,192 @@
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="61" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="0" t="n">
+      <c r="C2" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="61" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="61" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="61" t="n">
         <v>2</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="61" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="61" t="n">
         <v>3</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="61" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="61" t="n">
         <v>3</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="61" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="61" t="n">
         <v>2</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="61" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="61" t="n">
         <v>3</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="61" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="61" t="n">
         <v>3</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="61" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="61" t="n">
         <v>3</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="61" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="61" t="n">
         <v>3</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="61" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="61" t="n">
         <v>3</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="61" t="s">
         <v>71</v>
       </c>
     </row>
@@ -6252,366 +6262,366 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="61" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="61" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="61" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="61" t="n">
         <v>2</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="61" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="61" t="n">
         <v>3</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="61" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="D5" s="61" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" s="61" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E6" s="0" t="s">
+      <c r="D6" s="61" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" s="61" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E7" s="0" t="s">
+      <c r="D7" s="61" t="n">
+        <v>4</v>
+      </c>
+      <c r="E7" s="61" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E8" s="0" t="s">
+      <c r="D8" s="61" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" s="61" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E9" s="0" t="s">
+      <c r="D9" s="61" t="n">
+        <v>4</v>
+      </c>
+      <c r="E9" s="61" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="61" t="n">
         <v>3</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="61" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E11" s="0" t="s">
+      <c r="D11" s="61" t="n">
+        <v>4</v>
+      </c>
+      <c r="E11" s="61" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E12" s="0" t="s">
+      <c r="D12" s="61" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" s="61" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E13" s="0" t="s">
+      <c r="D13" s="61" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" s="61" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="61" t="n">
         <v>2</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="61" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="61" t="n">
         <v>2</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="61" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="61" t="n">
         <v>1</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" s="61" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="61" t="n">
         <v>2</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" s="61" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="61" t="n">
         <v>2</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" s="61" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="61" t="n">
         <v>2</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" s="61" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="61" t="n">
         <v>2</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="61" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="61" t="n">
         <v>2021</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="61" t="n">
         <v>2</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" s="61" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>